<commit_message>
implement testbase, read from excel, second test, testng.xml property files
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="7212"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,6 +21,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>Dan</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>syd2148</t>
+  </si>
+  <si>
+    <t>alerttest</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,14 +365,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement Common data provider, soft assertions, parameterization
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>firstname</t>
   </si>
@@ -48,6 +49,36 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Dan Car</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Tar</t>
+  </si>
+  <si>
+    <t>Pam</t>
+  </si>
+  <si>
+    <t>Sen</t>
+  </si>
+  <si>
+    <t>syd2143</t>
+  </si>
+  <si>
+    <t>syd2146</t>
   </si>
 </sst>
 </file>
@@ -365,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -401,6 +432,65 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement Runmode for Test suite level and test case level
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="7212"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="7212" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>firstname</t>
   </si>
@@ -45,9 +46,6 @@
     <t>syd2148</t>
   </si>
   <si>
-    <t>alerttest</t>
-  </si>
-  <si>
     <t>Customer added successfully</t>
   </si>
   <si>
@@ -79,6 +77,33 @@
   </si>
   <si>
     <t>syd2146</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>alerttext</t>
   </si>
 </sst>
 </file>
@@ -396,68 +421,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -466,6 +467,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -477,18 +561,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement for Jenkins parameters, reports and mail- via java
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="7212" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="7212"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>firstname</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>runmode</t>
@@ -423,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,10 +484,10 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -524,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>